<commit_message>
Part number updates in v0.3 and v0.4 BOMs
</commit_message>
<xml_diff>
--- a/reference/hardware/v0.3/v0.3.3_bom.xlsx
+++ b/reference/hardware/v0.3/v0.3.3_bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27815"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14360" windowHeight="16600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Full Kit" sheetId="1" r:id="rId1"/>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="243">
   <si>
     <t>QTY</t>
   </si>
@@ -270,21 +270,9 @@
     <t>RNF14FTD470RCT-ND</t>
   </si>
   <si>
-    <t>RES 2.49K OHM 0.25W 0.1% METAL FILM</t>
-  </si>
-  <si>
     <t>For GM Sensors</t>
   </si>
   <si>
-    <t>TT Electronics/Welwyn</t>
-  </si>
-  <si>
-    <t>RC55Y-2K49BI</t>
-  </si>
-  <si>
-    <t>985-1047-1-ND</t>
-  </si>
-  <si>
     <t>RES 3.9K OHM 1/4W 0.1% METAL FILM AXL</t>
   </si>
   <si>
@@ -354,9 +342,6 @@
     <t>Total of Materials:Cost to Manufacture</t>
   </si>
   <si>
-    <t>R1,3</t>
-  </si>
-  <si>
     <t>R7</t>
   </si>
   <si>
@@ -664,18 +649,6 @@
   </si>
   <si>
     <t>R10,13,21,23,24,50,51,57,58</t>
-  </si>
-  <si>
-    <t>PPC2.49KXCT-ND</t>
-  </si>
-  <si>
-    <t>RES 2.49K OHM 1/2W 1% AXIAL</t>
-  </si>
-  <si>
-    <t>Vishay BC Components</t>
-  </si>
-  <si>
-    <t>SFR16S0002491FR500</t>
   </si>
   <si>
     <t>D1,2,3,4</t>
@@ -851,6 +824,15 @@
   </si>
   <si>
     <t>969102-0000-DA</t>
+  </si>
+  <si>
+    <t>2.49k Ohm ±1% 0.25W, 1/4W Through Hole Resistor Axial Metal Film</t>
+  </si>
+  <si>
+    <t>MFR-25FBF52-2K49</t>
+  </si>
+  <si>
+    <t>2.49KXBK-ND</t>
   </si>
 </sst>
 </file>
@@ -1979,8 +1961,8 @@
   </sheetPr>
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I27" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2002,7 +1984,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2014,13 +1996,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -2029,7 +2011,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
@@ -2041,13 +2023,13 @@
         <v>10</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2080,13 +2062,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -2096,13 +2078,13 @@
         <v>16</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="K3" s="2" t="str">
         <f>VLOOKUP(I3,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -2135,13 +2117,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
@@ -2151,13 +2133,13 @@
         <v>16</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="K4" s="2" t="str">
         <f>VLOOKUP(I4,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -2190,13 +2172,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
@@ -2206,16 +2188,16 @@
         <v>16</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>237</v>
       </c>
       <c r="L5" s="27">
         <v>0.32</v>
@@ -2244,13 +2226,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -2260,16 +2242,16 @@
         <v>13</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="L6" s="27">
         <v>0.98</v>
@@ -2298,13 +2280,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>15</v>
@@ -2314,13 +2296,13 @@
         <v>13</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K7" s="2" t="str">
         <f>VLOOKUP(I7,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -2353,13 +2335,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>15</v>
@@ -2369,13 +2351,13 @@
         <v>16</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="K8" s="2" t="str">
         <f>VLOOKUP(I8,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -2408,13 +2390,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -2424,13 +2406,13 @@
         <v>16</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="K9" s="2" t="str">
         <f>VLOOKUP(I9,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -2463,13 +2445,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>15</v>
@@ -2479,13 +2461,13 @@
         <v>16</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="K10" s="2" t="str">
         <f>VLOOKUP(I10,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -2542,10 +2524,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>22</v>
@@ -2558,7 +2540,7 @@
         <v>24</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>25</v>
@@ -2597,32 +2579,32 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="L13" s="27">
         <v>0.36</v>
@@ -2651,30 +2633,30 @@
         <v>8</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="L14" s="27">
         <v>0.47</v>
@@ -2703,7 +2685,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>32</v>
@@ -2719,7 +2701,7 @@
         <v>29</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>34</v>
@@ -2785,7 +2767,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>36</v>
@@ -2801,7 +2783,7 @@
         <v>39</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>40</v>
@@ -2867,30 +2849,30 @@
         <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I19" s="3">
         <v>1935161</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="L19" s="26">
         <v>0.38</v>
@@ -2900,7 +2882,7 @@
         <v>5.32</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="O19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2920,28 +2902,28 @@
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="L20" s="27">
         <v>0.1</v>
@@ -2969,27 +2951,27 @@
         <v>6</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K21" s="2" t="e">
         <f>VLOOKUP(I21,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3050,29 +3032,29 @@
         <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
         <v>43</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="K23" s="2" t="str">
         <f>VLOOKUP(I23,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3129,13 +3111,13 @@
         <v>3</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -3143,16 +3125,16 @@
         <v>45</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="L25" s="27">
         <v>0.08</v>
@@ -3181,7 +3163,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>47</v>
@@ -3195,16 +3177,16 @@
         <v>45</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>50</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="L26" s="27">
         <v>0.06</v>
@@ -3233,30 +3215,30 @@
         <v>8</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C27" s="14">
         <v>680</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="L27" s="27">
         <v>0.22</v>
@@ -3266,7 +3248,7 @@
         <v>1.76</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="O27" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3287,7 +3269,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C28" s="3">
         <v>470</v>
@@ -3301,7 +3283,7 @@
         <v>52</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>53</v>
@@ -3322,15 +3304,15 @@
       </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(NOT(J28=""),A28&amp;","&amp;J28,"")</f>
         <v>6,RNF14FTD470RCT-ND</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(NOT(K28=""),K28&amp;"|"&amp;A28,"")</f>
         <v>279-LR1F470R|6</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" si="7"/>
+        <f>"Resistor - " &amp; A28&amp;"x "&amp;C28</f>
         <v>Resistor - 6x 470</v>
       </c>
     </row>
@@ -3339,51 +3321,50 @@
         <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>188</v>
+        <v>240</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3" t="s">
-        <v>189</v>
+        <v>45</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>190</v>
+        <v>241</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>187</v>
+        <v>242</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="L29" s="27">
-        <v>1.92</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M29" s="27">
-        <f t="shared" si="6"/>
-        <v>3.84</v>
-      </c>
-      <c r="N29" s="4"/>
+        <v>0.16</v>
+      </c>
+      <c r="N29" s="6"/>
       <c r="O29" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>2,PPC2.49KXCT-ND</v>
+        <f>IF(NOT(J29=""),A29&amp;","&amp;J29,"")</f>
+        <v>2,2.49KXBK-ND</v>
       </c>
       <c r="P29" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(NOT(K29=""),K29&amp;"|"&amp;A29,"")</f>
         <v>603-MFR-25FBF52-2K49|2</v>
       </c>
       <c r="Q29" t="str">
-        <f t="shared" si="7"/>
+        <f>"Resistor - " &amp; A29&amp;"x "&amp;C29</f>
         <v>Resistor - 2x 0.1% 2.49k</v>
       </c>
     </row>
@@ -3392,13 +3373,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -3406,13 +3387,13 @@
         <v>45</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K30" s="2" t="str">
         <f>VLOOKUP(I30,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3426,7 +3407,7 @@
         <v>0.3</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="O30" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3447,13 +3428,13 @@
         <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -3461,16 +3442,16 @@
         <v>45</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="L31" s="27">
         <v>0.1</v>
@@ -3499,13 +3480,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C32" s="3">
         <v>160</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -3513,13 +3494,13 @@
         <v>45</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K32" s="2" t="str">
         <f>VLOOKUP(I32,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3575,29 +3556,29 @@
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K34" s="2" t="str">
         <f>VLOOKUP(I34,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3629,32 +3610,32 @@
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="L35" s="27">
         <v>15.41</v>
@@ -3682,29 +3663,29 @@
         <v>2</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="K36" s="2" t="str">
         <f>VLOOKUP(I36,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3736,29 +3717,29 @@
         <v>1</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H37" s="31" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="J37" s="14" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="K37" s="2" t="str">
         <f>VLOOKUP(I37,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3790,23 +3771,23 @@
         <v>3</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="K38" s="2" t="str">
         <f>VLOOKUP(I38,'[1]Component List'!$L:$N,3,FALSE)</f>
@@ -3853,7 +3834,7 @@
         <v/>
       </c>
       <c r="P39" t="str">
-        <f t="shared" ref="P39:P83" si="8">IF(NOT(E39=""),E39&amp;"|"&amp;#REF!,"")</f>
+        <f t="shared" ref="P39" si="8">IF(NOT(E39=""),E39&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
@@ -3862,7 +3843,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -3884,7 +3865,7 @@
         <v/>
       </c>
       <c r="P40" t="str">
-        <f t="shared" ref="P40:P84" si="9">IF(NOT(E40=""),E40&amp;"|"&amp;#REF!,"")</f>
+        <f t="shared" ref="P40" si="9">IF(NOT(E40=""),E40&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
@@ -3908,14 +3889,14 @@
         <v/>
       </c>
       <c r="P41" t="str">
-        <f t="shared" ref="P41:P85" si="10">IF(NOT(E41=""),E41&amp;"|"&amp;#REF!,"")</f>
+        <f t="shared" ref="P41" si="10">IF(NOT(E41=""),E41&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -3934,7 +3915,7 @@
         <v/>
       </c>
       <c r="P42" t="str">
-        <f t="shared" ref="P42:P86" si="11">IF(NOT(E42=""),E42&amp;"|"&amp;#REF!,"")</f>
+        <f t="shared" ref="P42" si="11">IF(NOT(E42=""),E42&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
@@ -3943,20 +3924,20 @@
         <v>1</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -3973,7 +3954,7 @@
         <v/>
       </c>
       <c r="P43" t="str">
-        <f t="shared" ref="P43:P87" si="12">IF(NOT(E43=""),E43&amp;"|"&amp;#REF!,"")</f>
+        <f t="shared" ref="P43" si="12">IF(NOT(E43=""),E43&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
@@ -3982,7 +3963,7 @@
         <v>1</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -3992,7 +3973,7 @@
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
       <c r="J44" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="3">
@@ -4000,10 +3981,10 @@
       </c>
       <c r="M44" s="6"/>
       <c r="N44" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="P44" t="str">
-        <f t="shared" ref="P44:P88" si="13">IF(NOT(E44=""),E44&amp;"|"&amp;#REF!,"")</f>
+        <f t="shared" ref="P44" si="13">IF(NOT(E44=""),E44&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
@@ -4017,19 +3998,19 @@
       <c r="G45" s="4"/>
       <c r="H45" s="9"/>
       <c r="I45" s="33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J45" s="34"/>
       <c r="K45" s="32"/>
       <c r="L45" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M45" s="12">
         <f>SUM(M2:M44)</f>
-        <v>90.960000000000008</v>
+        <v>87.28</v>
       </c>
       <c r="N45" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P45" t="str">
         <f t="shared" ref="P45" si="14">IF(NOT(E45=""),E45&amp;"|"&amp;#REF!,"")</f>
@@ -4038,19 +4019,19 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P46" t="str">
-        <f t="shared" ref="P46:P90" si="15">IF(NOT(E46=""),E46&amp;"|"&amp;#REF!,"")</f>
+        <f t="shared" ref="P46" si="15">IF(NOT(E46=""),E46&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P47" t="str">
-        <f t="shared" ref="P47:P91" si="16">IF(NOT(E47=""),E47&amp;"|"&amp;#REF!,"")</f>
+        <f t="shared" ref="P47" si="16">IF(NOT(E47=""),E47&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P48" t="str">
-        <f t="shared" ref="P48:P92" si="17">IF(NOT(E48=""),E48&amp;"|"&amp;#REF!,"")</f>
+        <f t="shared" ref="P48" si="17">IF(NOT(E48=""),E48&amp;"|"&amp;#REF!,"")</f>
         <v/>
       </c>
     </row>
@@ -4065,13 +4046,13 @@
     <hyperlink ref="J13" r:id="rId2" display="1N5818-TPCT-ND"/>
     <hyperlink ref="J17" r:id="rId3"/>
     <hyperlink ref="J25" r:id="rId4" display="10.0KXBK-ND"/>
-    <hyperlink ref="J29" r:id="rId5" display="985-1047-1-ND"/>
-    <hyperlink ref="J30" r:id="rId6"/>
-    <hyperlink ref="J31" r:id="rId7"/>
-    <hyperlink ref="J35" r:id="rId8"/>
-    <hyperlink ref="J3" r:id="rId9" display="478-1842-ND"/>
-    <hyperlink ref="J7" r:id="rId10" display="445-5312-ND"/>
-    <hyperlink ref="J8" r:id="rId11" display="399-4148-ND"/>
+    <hyperlink ref="J30" r:id="rId5"/>
+    <hyperlink ref="J31" r:id="rId6"/>
+    <hyperlink ref="J35" r:id="rId7"/>
+    <hyperlink ref="J3" r:id="rId8" display="478-1842-ND"/>
+    <hyperlink ref="J7" r:id="rId9" display="445-5312-ND"/>
+    <hyperlink ref="J8" r:id="rId10" display="399-4148-ND"/>
+    <hyperlink ref="J29" r:id="rId11" display="985-1047-1-ND"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="35" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4086,8 +4067,8 @@
   </sheetPr>
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:XFD37"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4110,7 +4091,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -4122,13 +4103,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
@@ -4149,10 +4130,10 @@
         <v>10</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4185,13 +4166,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -4201,16 +4182,16 @@
         <v>4</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="L3" s="5">
         <v>1.7</v>
@@ -4235,13 +4216,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
@@ -4251,16 +4232,16 @@
         <v>15</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="L4" s="5">
         <v>0.66</v>
@@ -4285,13 +4266,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
@@ -4301,16 +4282,16 @@
         <v>17</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="L5" s="5">
         <v>0.32</v>
@@ -4335,13 +4316,13 @@
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>12</v>
@@ -4351,16 +4332,16 @@
         <v>2</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="L6" s="5">
         <v>1.57</v>
@@ -4385,13 +4366,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>15</v>
@@ -4401,16 +4382,16 @@
         <v>2</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="L7" s="5">
         <v>0.62</v>
@@ -4435,13 +4416,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>15</v>
@@ -4451,16 +4432,16 @@
         <v>3</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="L8" s="5">
         <v>0.24</v>
@@ -4485,13 +4466,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -4501,16 +4482,16 @@
         <v>4</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="L9" s="5">
         <v>0.66</v>
@@ -4535,13 +4516,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>15</v>
@@ -4549,16 +4530,16 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L10" s="5">
         <v>0.25</v>
@@ -4603,10 +4584,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>22</v>
@@ -4619,7 +4600,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>24</v>
@@ -4653,10 +4634,10 @@
         <v>4</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>28</v>
@@ -4669,7 +4650,7 @@
         <v>18</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>29</v>
@@ -4703,26 +4684,26 @@
         <v>4</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="L14" s="5">
         <v>0.47</v>
@@ -4747,7 +4728,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>32</v>
@@ -4763,7 +4744,7 @@
         <v>13</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>29</v>
@@ -4820,7 +4801,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>36</v>
@@ -4836,7 +4817,7 @@
         <v>1</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>39</v>
@@ -4893,28 +4874,28 @@
         <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="L19" s="3">
         <v>0.40200000000000002</v>
@@ -4924,7 +4905,7 @@
         <v>5.6280000000000001</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="O19" s="4" t="str">
         <f t="shared" si="2"/>
@@ -4940,24 +4921,24 @@
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="L20" s="5">
         <v>0.1</v>
@@ -4981,13 +4962,13 @@
         <v>5</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -4995,16 +4976,16 @@
         <v>1</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="L21" s="6">
         <v>0.56000000000000005</v>
@@ -5052,32 +5033,32 @@
         <v>6</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3">
         <v>8</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>43</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L23" s="6">
         <v>1.51</v>
@@ -5122,13 +5103,13 @@
         <v>3</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -5136,7 +5117,7 @@
         <v>7</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>45</v>
@@ -5145,7 +5126,7 @@
         <v>46</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="L25" s="5">
         <v>0.08</v>
@@ -5170,7 +5151,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>47</v>
@@ -5184,7 +5165,7 @@
         <v>32</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I26" s="3" t="s">
         <v>45</v>
@@ -5218,26 +5199,26 @@
         <v>4</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C27" s="14">
         <v>680</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="J27" s="7"/>
       <c r="K27" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="L27" s="15">
         <v>0.22</v>
@@ -5247,7 +5228,7 @@
         <v>0.88</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="O27" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5264,7 +5245,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C28" s="3">
         <v>470</v>
@@ -5278,7 +5259,7 @@
         <v>9</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>52</v>
@@ -5306,50 +5287,48 @@
         <v>Resistor - 6x 470</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="40" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="20">
-        <f>LEN(B29)-LEN(SUBSTITUTE(B29,",",""))+1</f>
         <v>2</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>83</v>
+        <v>203</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="F29" s="3"/>
-      <c r="G29" s="3">
-        <v>3</v>
+      <c r="G29" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>58</v>
+        <v>241</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>242</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="L29" s="5">
-        <v>1.92</v>
-      </c>
-      <c r="M29" s="6">
-        <f t="shared" si="5"/>
-        <v>3.84</v>
-      </c>
-      <c r="N29" s="4"/>
+        <v>234</v>
+      </c>
+      <c r="L29" s="27">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M29" s="27">
+        <v>0.16</v>
+      </c>
+      <c r="N29" s="6"/>
       <c r="O29" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>2,985-1047-1-ND</v>
+        <f>IF(NOT(J29=""),A29&amp;","&amp;J29,"")</f>
+        <v>2,2.49KXBK-ND</v>
       </c>
       <c r="P29" t="str">
         <f t="shared" si="6"/>
@@ -5361,13 +5340,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -5375,16 +5354,16 @@
         <v>1</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L30" s="5">
         <v>0.46</v>
@@ -5394,7 +5373,7 @@
         <v>0.46</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="O30" s="4" t="str">
         <f t="shared" si="2"/>
@@ -5411,13 +5390,13 @@
         <v>8</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -5425,16 +5404,16 @@
         <v>17</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="L31" s="5">
         <v>0.1</v>
@@ -5459,13 +5438,13 @@
         <v>2</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C32" s="3">
         <v>160</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -5473,16 +5452,16 @@
         <v>4</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>45</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="L32" s="5">
         <v>0.27</v>
@@ -5526,32 +5505,32 @@
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3">
         <v>2</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L34" s="5">
         <v>1.68</v>
@@ -5575,16 +5554,16 @@
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3">
@@ -5592,11 +5571,11 @@
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="J35" s="3"/>
       <c r="K35" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L35" s="6">
         <v>15.41</v>
@@ -5620,30 +5599,30 @@
         <v>1</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F36" s="14"/>
       <c r="G36" s="14">
         <v>2</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="L36" s="22">
         <v>2.92</v>
@@ -5667,30 +5646,30 @@
         <v>1</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="J37" s="14" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="K37" s="14" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="L37" s="22">
         <v>2.4</v>
@@ -5714,24 +5693,24 @@
         <v>3</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="L38" s="6">
         <v>0.5</v>
@@ -5775,7 +5754,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -5822,7 +5801,7 @@
     <row r="42" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -5846,10 +5825,10 @@
         <v>1</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
@@ -5859,10 +5838,10 @@
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J43" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="6">
@@ -5883,7 +5862,7 @@
         <v>1</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -5894,14 +5873,14 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="L44" s="3">
         <v>61.65</v>
       </c>
       <c r="M44" s="6"/>
       <c r="N44" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -5915,18 +5894,18 @@
       <c r="H45" s="9"/>
       <c r="I45" s="4"/>
       <c r="J45" s="33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="K45" s="34"/>
       <c r="L45" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M45" s="12">
         <f>SUM(M2:M44)</f>
-        <v>80.337999999999994</v>
+        <v>76.657999999999987</v>
       </c>
       <c r="N45" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -5942,11 +5921,11 @@
     <hyperlink ref="K13" r:id="rId4"/>
     <hyperlink ref="K17" r:id="rId5"/>
     <hyperlink ref="K25" r:id="rId6" display="10.0KXBK-ND"/>
-    <hyperlink ref="K29" r:id="rId7"/>
-    <hyperlink ref="K30" r:id="rId8"/>
-    <hyperlink ref="K31" r:id="rId9"/>
-    <hyperlink ref="K35" r:id="rId10"/>
-    <hyperlink ref="K6" r:id="rId11" display="478-1910-ND"/>
+    <hyperlink ref="K30" r:id="rId7"/>
+    <hyperlink ref="K31" r:id="rId8"/>
+    <hyperlink ref="K35" r:id="rId9"/>
+    <hyperlink ref="K6" r:id="rId10" display="478-1910-ND"/>
+    <hyperlink ref="J29" r:id="rId11" display="985-1047-1-ND"/>
   </hyperlinks>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="34" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>